<commit_message>
Updated test xlsx file
Modified test file for consistency
</commit_message>
<xml_diff>
--- a/tests/test_files/test.xlsx
+++ b/tests/test_files/test.xlsx
@@ -4137,7 +4137,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Added test based on known data
</commit_message>
<xml_diff>
--- a/tests/test_files/test.xlsx
+++ b/tests/test_files/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Bars1_2_3_Snd" sheetId="8" r:id="rId9"/>
     <sheet name="Bars4_5_6_7_8_Snd" sheetId="9" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -292,8 +292,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,7 +414,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -449,7 +448,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -625,16 +623,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -645,7 +643,7 @@
         <v>42199</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -656,12 +654,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -669,7 +667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -683,7 +681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -697,7 +695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -711,12 +709,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -730,12 +728,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -743,7 +741,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -760,7 +758,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -786,7 +784,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -806,7 +804,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>99</v>
       </c>
@@ -847,14 +845,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N46"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -868,7 +868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -882,12 +882,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="I4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -895,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -946,12 +946,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="J9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -968,12 +968,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -993,7 +993,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -1013,7 +1013,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="F15" t="s">
         <v>49</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="I16" t="s">
         <v>52</v>
       </c>
@@ -1050,12 +1050,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14">
       <c r="N17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14">
       <c r="E18" t="s">
         <v>23</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14">
       <c r="B20">
         <v>40</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>-7.3</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14">
       <c r="B21">
         <v>41</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>-6.7</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14">
       <c r="B22">
         <v>42</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14">
       <c r="B23">
         <v>43</v>
       </c>
@@ -1248,7 +1248,7 @@
         <v>-5.4</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14">
       <c r="B24">
         <v>44</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>-6.5</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14">
       <c r="B25">
         <v>45</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14">
       <c r="B26">
         <v>59</v>
       </c>
@@ -1371,7 +1371,7 @@
         <v>-5.8</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14">
       <c r="B27">
         <v>60</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>-6.6</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14">
       <c r="B28">
         <v>65</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14">
       <c r="B29">
         <v>66</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>-6.7</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14">
       <c r="B30">
         <v>67</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>-5.9</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14">
       <c r="B31">
         <v>68</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>-5.7</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14">
       <c r="B32">
         <v>69</v>
       </c>
@@ -1617,7 +1617,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14">
       <c r="B33">
         <v>74</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14">
       <c r="B34">
         <v>75</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14">
       <c r="B35">
         <v>76</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14">
       <c r="B36">
         <v>53</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>-5.6</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14">
       <c r="B37">
         <v>54</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>-7</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:14">
       <c r="B38">
         <v>55</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14">
       <c r="B40" t="s">
         <v>56</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14">
       <c r="E41" t="s">
         <v>59</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:14">
       <c r="E42" t="s">
         <v>62</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14">
       <c r="B44" t="s">
         <v>63</v>
       </c>
@@ -1913,7 +1913,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14">
       <c r="B45" t="s">
         <v>64</v>
       </c>
@@ -1930,7 +1930,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:14">
       <c r="B46" t="s">
         <v>65</v>
       </c>
@@ -1953,14 +1953,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>42200</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -1982,12 +1982,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -2037,12 +2037,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -2056,12 +2056,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>131</v>
       </c>
@@ -2167,7 +2167,7 @@
         <v>57.5</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19">
         <v>103</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>55.7</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20">
         <v>102</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>57.1</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12">
       <c r="B21">
         <v>101</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>57.4</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12">
       <c r="B22">
         <v>100</v>
       </c>
@@ -2313,14 +2313,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>42199</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -2342,12 +2342,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -2383,7 +2383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -2397,12 +2397,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -2416,12 +2416,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -2472,7 +2472,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -2492,7 +2492,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>132</v>
       </c>
@@ -2533,14 +2533,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>42199</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -2562,12 +2562,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -2617,12 +2617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -2636,12 +2636,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -2692,7 +2692,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>59</v>
       </c>
@@ -2747,7 +2747,7 @@
         <v>57.3</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19">
         <v>60</v>
       </c>
@@ -2788,14 +2788,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>42199</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -2817,12 +2817,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -2844,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -2872,12 +2872,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -2891,12 +2891,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -2904,7 +2904,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -2921,7 +2921,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -2967,7 +2967,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>40</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>46.8</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19">
         <v>41</v>
       </c>
@@ -3037,7 +3037,7 @@
         <v>53.3</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20">
         <v>42</v>
       </c>
@@ -3078,14 +3078,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:M20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -3096,7 +3101,7 @@
         <v>42199</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -3107,12 +3112,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3120,7 +3125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -3134,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -3148,7 +3153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -3162,12 +3167,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -3181,12 +3186,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -3194,7 +3199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -3211,7 +3216,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -3237,7 +3242,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -3257,7 +3262,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18">
         <v>43</v>
       </c>
@@ -3295,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:13">
       <c r="B19">
         <v>44</v>
       </c>
@@ -3333,7 +3338,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20">
         <v>45</v>
       </c>
@@ -3377,14 +3382,16 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -3395,7 +3402,7 @@
         <v>42199</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -3406,12 +3413,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3419,7 +3426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -3433,7 +3440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -3447,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -3461,12 +3468,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -3480,12 +3487,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -3493,7 +3500,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -3510,7 +3517,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -3536,7 +3543,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -3556,7 +3563,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>75</v>
       </c>
@@ -3591,7 +3598,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19">
         <v>68</v>
       </c>
@@ -3626,7 +3633,7 @@
         <v>46.3</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20">
         <v>69</v>
       </c>
@@ -3661,7 +3668,7 @@
         <v>43.2</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12">
       <c r="B21">
         <v>76</v>
       </c>
@@ -3696,7 +3703,7 @@
         <v>41.9</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12">
       <c r="B22">
         <v>65</v>
       </c>
@@ -3731,7 +3738,7 @@
         <v>55.2</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12">
       <c r="B23">
         <v>66</v>
       </c>
@@ -3766,7 +3773,7 @@
         <v>52.1</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12">
       <c r="B24">
         <v>67</v>
       </c>
@@ -3801,7 +3808,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12">
       <c r="B25">
         <v>74</v>
       </c>
@@ -3842,16 +3849,16 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:12">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -3862,7 +3869,7 @@
         <v>42199</v>
       </c>
     </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:12">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -3873,12 +3880,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12">
       <c r="J4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:12">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -3886,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:12">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -3900,7 +3907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:12">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -3914,7 +3921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:12">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -3928,12 +3935,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:12">
       <c r="B9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:12">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -3947,12 +3954,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:12">
       <c r="B12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:12">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -3960,7 +3967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:12">
       <c r="D14" t="s">
         <v>14</v>
       </c>
@@ -3977,7 +3984,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:12">
       <c r="D15" t="s">
         <v>19</v>
       </c>
@@ -4003,7 +4010,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:12">
       <c r="D16" t="s">
         <v>23</v>
       </c>
@@ -4023,7 +4030,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12">
       <c r="B18">
         <v>55</v>
       </c>
@@ -4058,7 +4065,7 @@
         <v>48.7</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12">
       <c r="B19">
         <v>54</v>
       </c>
@@ -4093,7 +4100,7 @@
         <v>49.3</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12">
       <c r="B20">
         <v>53</v>
       </c>
@@ -4134,16 +4141,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -4157,7 +4164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14">
       <c r="B3" t="s">
         <v>86</v>
       </c>
@@ -4171,12 +4178,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="I4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -4184,7 +4191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>4</v>
       </c>
@@ -4201,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>5</v>
       </c>
@@ -4218,7 +4225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -4235,12 +4242,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="J9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14">
       <c r="B10" t="s">
         <v>9</v>
       </c>
@@ -4257,12 +4264,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" t="s">
         <v>12</v>
       </c>
@@ -4282,7 +4289,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="E14" t="s">
         <v>19</v>
       </c>
@@ -4302,7 +4309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="F15" t="s">
         <v>49</v>
       </c>
@@ -4331,7 +4338,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="I16" t="s">
         <v>52</v>
       </c>
@@ -4339,12 +4346,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14">
       <c r="N17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14">
       <c r="E18" t="s">
         <v>23</v>
       </c>
@@ -4373,7 +4380,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14">
       <c r="B20">
         <v>96</v>
       </c>
@@ -4414,7 +4421,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14">
       <c r="B21">
         <v>99</v>
       </c>
@@ -4455,7 +4462,7 @@
         <v>-6.9</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14">
       <c r="B22">
         <v>100</v>
       </c>
@@ -4496,7 +4503,7 @@
         <v>-4.7</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14">
       <c r="B23">
         <v>101</v>
       </c>
@@ -4537,7 +4544,7 @@
         <v>-6.2</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14">
       <c r="B24">
         <v>102</v>
       </c>
@@ -4578,7 +4585,7 @@
         <v>-6.8</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14">
       <c r="B25">
         <v>103</v>
       </c>
@@ -4619,7 +4626,7 @@
         <v>-7.3</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14">
       <c r="B26">
         <v>104</v>
       </c>
@@ -4660,7 +4667,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14">
       <c r="B27">
         <v>105</v>
       </c>
@@ -4701,7 +4708,7 @@
         <v>-7.5</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14">
       <c r="B28">
         <v>106</v>
       </c>
@@ -4742,7 +4749,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14">
       <c r="B29">
         <v>107</v>
       </c>
@@ -4783,7 +4790,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14">
       <c r="B30">
         <v>108</v>
       </c>
@@ -4824,7 +4831,7 @@
         <v>-7.5</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14">
       <c r="B31">
         <v>118</v>
       </c>
@@ -4865,7 +4872,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14">
       <c r="B32">
         <v>119</v>
       </c>
@@ -4906,7 +4913,7 @@
         <v>-7.3</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:14">
       <c r="B33">
         <v>120</v>
       </c>
@@ -4947,7 +4954,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:14">
       <c r="B34">
         <v>121</v>
       </c>
@@ -4988,7 +4995,7 @@
         <v>-7.3</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:14">
       <c r="B35">
         <v>122</v>
       </c>
@@ -5029,7 +5036,7 @@
         <v>-7.2</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:14">
       <c r="B36">
         <v>131</v>
       </c>
@@ -5070,7 +5077,7 @@
         <v>-7.4</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:14">
       <c r="B37">
         <v>132</v>
       </c>
@@ -5111,7 +5118,7 @@
         <v>-6.1</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:14">
       <c r="B39" t="s">
         <v>56</v>
       </c>
@@ -5122,7 +5129,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:14">
       <c r="E40" t="s">
         <v>59</v>
       </c>
@@ -5133,7 +5140,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:14">
       <c r="E41" t="s">
         <v>62</v>
       </c>
@@ -5144,7 +5151,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:14">
       <c r="B43" t="s">
         <v>63</v>
       </c>
@@ -5161,7 +5168,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:14">
       <c r="B44" t="s">
         <v>64</v>
       </c>
@@ -5178,7 +5185,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:14">
       <c r="B45" t="s">
         <v>65</v>
       </c>

</xml_diff>